<commit_message>
Wrote design brief. Worked up pen-and-paper approach.
</commit_message>
<xml_diff>
--- a/Design Brief and Analysis/SnapperCodingChallengeDesignDocument.xlsx
+++ b/Design Brief and Analysis/SnapperCodingChallengeDesignDocument.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcox\Desktop\git\SnapperCodingChallenge\Design Brief and Analysis\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AB2710-61FD-470B-9C51-29A96DE0F957}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="23625" yWindow="7590" windowWidth="7500" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,11 +24,27 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t xml:space="preserve">Snapper Coding Challenge </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -49,8 +71,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -66,6 +89,646 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>235323</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B201F95E-1E8F-436B-9871-63A0A97E74E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="171450" y="679076"/>
+          <a:ext cx="4299697" cy="2895600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1"/>
+            <a:t>Brief </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="1"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0"/>
+            <a:t>Design</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+            <a:t> an application that scans an arbitrarily sized grid of fuzzy data containing "Torpedooes" and "Starships".  The shape of these objects is described in the "NuclearTorpedo.blf" and "Starship.blf" files. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+            <a:t>The following should  be returned: </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+            <a:t>1. Type of target found </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+            <a:t>2. Co-ordinates of the target on the snapper data </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+            <a:t>3. Indication of confidence (defined by number of grid elements that are correct/number of total grid elements that make up the star ship."</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="sng" baseline="0"/>
+            <a:t>Bonus: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>Let the console paplication print the grid which have highlighted the areas in yellow that are Torpedos and Starships, and print the data as a nice summary. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>247314</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>37833</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5557F86-7DAE-4956-97BC-DC1E156A3E06}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4876800" y="904875"/>
+          <a:ext cx="2685714" cy="2133333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>56030</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{978D5027-571B-4195-8AB6-F799B80FD0BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="190500" y="3669926"/>
+          <a:ext cx="4273924" cy="3770780"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1"/>
+            <a:t>Approach 1 - Brute Force Method </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="1"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" u="sng">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Manual Approach/Pen</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" u="sng" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> and Paper </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100" b="1" u="sng">
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0"/>
+            <a:t>Print</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+            <a:t> out the raw snapper data as a grid. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="sng" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="sng" baseline="0"/>
+            <a:t>Foreach object e.g. torpedo or starship</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>     Get the "size" of the object, i.e. m*n rectangle that envelopes the shape.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>     Count the number of objects that need to be compared (i.e. number of pluses in    the grid =&gt; this should be stored as a static property to stop repeated calls when the object is instantiated</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>    Note down the elements as i,j values that need to be compared, ignoring the white space as a result of the m*n enveloping rectangle. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>     Break down the raw snapper data grid into overlapping slices "m*n" that overlap </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="sng" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="sng" baseline="0"/>
+            <a:t>          For each of the relevant elements, check if theyre a plus. If so     count them .</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>   Compare count of pluses to count of pluses that should be there. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>   Return confidence of target and coordinate of target found      </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>	</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="sng" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>72838</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>110938</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69144D7E-2E9E-43FC-BC1C-2DAE0CAD3506}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4840941" y="3647514"/>
+          <a:ext cx="4273924" cy="2895600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1"/>
+            <a:t>NOTES:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="1" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>1. To optimise the speed of the programme, we must stored important properties as static when each shape is instantiated e.g. number of elements to be checked etc. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>112568</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>73348</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7974F4C-C66F-44D6-8630-3454F7C52AE8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="190500" y="7490113"/>
+          <a:ext cx="4281055" cy="3770780"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" u="sng">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Manual Approach/Pen</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" u="sng" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> and Paper </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100" b="1" u="sng">
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0"/>
+            <a:t>Print</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+            <a:t> out the raw snapper data as a grid. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="sng" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="sng" baseline="0"/>
+            <a:t>Foreach object e.g. torpedo or starship</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>     Get the "size" of the object, i.e. m*n rectangle that envelopes the shape.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>     Count the number of objects that need to be compared (i.e. number of pluses in    the grid =&gt; this should be stored as a static property to stop repeated calls when the object is instantiated</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>    Note down the elements as i,j values that need to be compared, ignoring the white space as a result of the m*n enveloping rectangle. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>     Break down the raw snapper data grid into overlapping slices "m*n" that overlap </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="sng" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="sng" baseline="0"/>
+            <a:t>          For each of the relevant elements, check if theyre a plus. If so     count them .</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>   Compare count of pluses to count of pluses that should be there. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>   Return confidence of target and coordinate of target found      </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>	</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="sng" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +993,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="N51" sqref="N51"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Defined procedural method of carrying out the task.
</commit_message>
<xml_diff>
--- a/Design Brief and Analysis/SnapperCodingChallengeDesignDocument.xlsx
+++ b/Design Brief and Analysis/SnapperCodingChallengeDesignDocument.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcox\Desktop\git\SnapperCodingChallenge\Design Brief and Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AB2710-61FD-470B-9C51-29A96DE0F957}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB6A11A-5BA2-40E7-B056-76693A0F7D60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23625" yWindow="7590" windowWidth="7500" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,16 +25,131 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">Snapper Coding Challenge </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Methods we Need </t>
+  </si>
+  <si>
+    <t>{Convert the target txtfile into a 2d array of characters}</t>
+  </si>
+  <si>
+    <t>static array[char]char[] ConvertTxtFileTo2DArray(string txtfile)</t>
+  </si>
+  <si>
+    <t>static List&lt;Tuple&lt;x,y&gt;&gt; GetCoordinatesToBeConsideredWithin2DArray</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given a 2D matrix return a list of tuples(x,y) that define coords </t>
+  </si>
+  <si>
+    <t>within the matrix that will be used later to verify whether a slice</t>
+  </si>
+  <si>
+    <t>does indeed contain a spaceship etc</t>
+  </si>
+  <si>
+    <t>{We should also provide a method to strip out any blank columns or rows</t>
+  </si>
+  <si>
+    <r>
+      <t>static Bool Compare2DMatrices(Array[char,char]</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Array[char][char] </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">sliceToCheck, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">List&lt;Tuple&lt;x,y&gt;&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">coordsToCheck, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>double</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> accuracy (e.g. 0.5 = 50% will yield a match. </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Author: Peter Cox </t>
+  </si>
+  <si>
+    <t>Source Code: https://github.com/EurocodeHelpers/SnapperCodingChallenge</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -44,6 +159,46 @@
     </font>
     <font>
       <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -71,9 +226,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -97,13 +257,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>235323</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -155,9 +315,41 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1"/>
-            <a:t>Brief </a:t>
-          </a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" u="sng">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Design Brief</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" u="sng" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" b="1">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-GB" sz="1100" b="1"/>
@@ -241,13 +433,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>247314</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>152064</xdr:colOff>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>37833</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -285,14 +477,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>56030</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -307,8 +499,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="190500" y="3669926"/>
-          <a:ext cx="4273924" cy="3770780"/>
+          <a:off x="190500" y="3476625"/>
+          <a:ext cx="4305300" cy="3400425"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -343,15 +535,6 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1"/>
-            <a:t>Approach 1 - Brute Force Method </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="1"/>
-        </a:p>
-        <a:p>
-          <a:r>
             <a:rPr lang="en-GB" sz="1100" b="1" u="sng">
               <a:solidFill>
                 <a:srgbClr val="0070C0"/>
@@ -472,14 +655,14 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>72838</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>110938</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>149678</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -494,8 +677,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4840941" y="3647514"/>
-          <a:ext cx="4273924" cy="2895600"/>
+          <a:off x="4898571" y="3461017"/>
+          <a:ext cx="5031922" cy="3124840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -531,8 +714,13 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="1"/>
-            <a:t>NOTES:</a:t>
-          </a:r>
+            <a:t>QUESTIONS/NOTES:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100" b="1"/>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-GB" sz="1100" b="1" u="none" baseline="0"/>
@@ -542,6 +730,51 @@
             <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
             <a:t>1. To optimise the speed of the programme, we must stored important properties as static when each shape is instantiated e.g. number of elements to be checked etc. </a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>2. Should we use 2d-array [][] or jagged array [,] - working with rectangular objects so 2d-array will be used as no need for flexibility of width of rows etc. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>3. We should error handle to catch when grid not rectangular and there are errors. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>4. The objects contain empty white columns and rows - we should trim these out to optimise the algorithm. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>5. What happens if the input files contains other non "X" or white-space ASCII characters? Do we want tight or loose exception handling - e.g. return errror message if contaisn non "X" characters, or simply run through analysis and assume that if not X, not counted as data. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>6. Do a simple method for a grid of say 4 1's within 16*16 grid as a practice!</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>7. The application make get duplicates e.g. adding 1 to column especially if logic very fuzzy - how to cater for this? </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>8. How are the "co-ordinates" of the ITarget defined? </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-GB" sz="1100" b="1"/>
@@ -553,15 +786,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>112568</xdr:rowOff>
+      <xdr:rowOff>179243</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>73348</xdr:rowOff>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -576,8 +809,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="190500" y="7490113"/>
-          <a:ext cx="4281055" cy="3770780"/>
+          <a:off x="200025" y="6992419"/>
+          <a:ext cx="4273924" cy="5726257"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -617,7 +850,7 @@
                 <a:srgbClr val="0070C0"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Manual Approach/Pen</a:t>
+            <a:t>Procedural/Non-OOP Approach (Initially only</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="1" u="sng" baseline="0">
@@ -625,8 +858,10 @@
                 <a:srgbClr val="0070C0"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> and Paper </a:t>
-          </a:r>
+            <a:t> consider the starship).</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="en-GB" sz="1100" b="1" u="sng">
             <a:solidFill>
               <a:srgbClr val="0070C0"/>
@@ -634,89 +869,689 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0"/>
-            <a:t>Print</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-            <a:t> out the raw snapper data as a grid. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="sng" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" u="sng" baseline="0"/>
-            <a:t>Foreach object e.g. torpedo or starship</a:t>
-          </a:r>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="sng" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Pre-Processing </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="sng" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1. Convert the following raw snapper data as an input file into an array[char][char].</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>2. Convert the StarshipData input file into an array[char][char] enveloping the extents of the object, making sure to trim any empty rows, </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>3. Obtain the elements of the starship array[char]char[] that are within the perimeter of the object {X,Y} =&gt; we could use a tuple to present this or a struct. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="sng" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="sng" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Processing</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1. Break down the map data into a series of slices =&gt; use the Compare2DMatrices method to determine whether a starship is contained within the slice/submatrix for each slice based on assumption that a match &gt;50% means that a starship has been detected. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="sng" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Post-Processing </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1. Print to console when a starship has been detected, along with its coordinates and target accuracy =&gt; the coordinates should be defined as the centroid of the 2D Array </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>2. (If get time =&gt; print out the map, and shade in yellow where a spaceship has been identified and orange for nuclear torpedeoes for fun). </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" u="none">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="1" u="none">
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="1" u="sng">
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
         </a:p>
         <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
-            <a:t>     Get the "size" of the object, i.e. m*n rectangle that envelopes the shape.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
-            <a:t>     Count the number of objects that need to be compared (i.e. number of pluses in    the grid =&gt; this should be stored as a static property to stop repeated calls when the object is instantiated</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
-            <a:t>    Note down the elements as i,j values that need to be compared, ignoring the white space as a result of the m*n enveloping rectangle. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
-            <a:t>     Break down the raw snapper data grid into overlapping slices "m*n" that overlap </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="sng" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" u="sng" baseline="0"/>
-            <a:t>          For each of the relevant elements, check if theyre a plus. If so     count them .</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
-            <a:t>   Compare count of pluses to count of pluses that should be there. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
-            <a:t>   Return confidence of target and coordinate of target found      </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
           <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
-            <a:t>	</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="sng" baseline="0"/>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
@@ -994,18 +1829,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N51" sqref="N51"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N67" sqref="N67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="19.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+    </row>
+    <row r="2" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A2" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A3" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="39" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I39" s="2"/>
+    </row>
+    <row r="40" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I40" s="2"/>
+    </row>
+    <row r="41" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I41" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I43" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I44" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I47" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I48" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I49" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I50" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I52" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I54" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Deleted and unzipped starting files.
</commit_message>
<xml_diff>
--- a/Design Brief and Analysis/SnapperCodingChallengeDesignDocument.xlsx
+++ b/Design Brief and Analysis/SnapperCodingChallengeDesignDocument.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcox\Desktop\git\SnapperCodingChallenge\Design Brief and Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97334F0-1730-4CD8-870A-A1772CCA5DD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041E797C-D83F-430C-B095-F2A29BB5E334}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t xml:space="preserve">Snapper Coding Challenge </t>
   </si>
@@ -145,10 +145,13 @@
     <t>Source Code: https://github.com/EurocodeHelpers/SnapperCodingChallenge</t>
   </si>
   <si>
-    <t>static array[char]char[] ConvertTxtFileTo2DArray_Compressed(string txtfile)</t>
+    <t xml:space="preserve">As above, but this time we should strip out any blank rows or columns. </t>
   </si>
   <si>
-    <t xml:space="preserve">As above, but this time we should strip out any blank rows or columns. </t>
+    <t>static array[char]char[] TrimArray(char[,] array)</t>
+  </si>
+  <si>
+    <t>DONE!</t>
   </si>
 </sst>
 </file>
@@ -1011,6 +1014,65 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" u="none" strike="sngStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>2. Convert the StarshipData input file into an array[char][char] enveloping the extents of the object, making sure to trim any empty rows, </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
             <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
@@ -1020,66 +1082,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>2. Trim out any blank </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>2. Convert the StarshipData input file into an array[char][char] enveloping the extents of the object, making sure to trim any empty rows, </a:t>
+            <a:t>3. Obtain a list of the elements within the shape that we need to compare against the slice of the array =&gt; lets use a Tuple&lt;x,y&gt;</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1894,10 +1897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:P55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50:I55"/>
+      <selection activeCell="O58" sqref="O58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1923,40 +1926,46 @@
     <row r="4" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
     </row>
-    <row r="39" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I39" s="2"/>
     </row>
-    <row r="40" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I40" s="2"/>
     </row>
-    <row r="41" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I41" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I43" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="P43" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="44" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I44" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I47" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="P47" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="48" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I48" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="50" spans="9:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ticked off todo items in design doc.
</commit_message>
<xml_diff>
--- a/Design Brief and Analysis/SnapperCodingChallengeDesignDocument.xlsx
+++ b/Design Brief and Analysis/SnapperCodingChallengeDesignDocument.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcox\Desktop\git\SnapperCodingChallenge\Design Brief and Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041E797C-D83F-430C-B095-F2A29BB5E334}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9554C22-758A-4CA3-813D-09C202679C32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t xml:space="preserve">Snapper Coding Challenge </t>
   </si>
@@ -153,6 +153,9 @@
   <si>
     <t>DONE!</t>
   </si>
+  <si>
+    <t>`</t>
+  </si>
 </sst>
 </file>
 
@@ -215,12 +218,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -235,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -243,6 +252,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1073,66 +1088,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>3. Obtain a list of the elements within the shape that we need to compare against the slice of the array =&gt; lets use a Tuple&lt;x,y&gt;</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
+            <a:rPr lang="en-GB" sz="1100" b="1" u="none" strike="sngStrike" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -1221,6 +1177,93 @@
             <a:tabLst/>
             <a:defRPr/>
           </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" b="1" u="none" strike="sngStrike" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" u="none" strike="sngStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1. Write a method to compare a given matrix with another matrix, comparing ONLY against a given list of co-ordinates</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
           <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
             <a:solidFill>
               <a:schemeClr val="dk1"/>
@@ -1629,6 +1672,50 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>462306</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20AADD9B-62CC-42D4-88BF-E4D5DDBE6DA9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10695214" y="4789714"/>
+          <a:ext cx="16804485" cy="8191500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1897,10 +1984,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P55"/>
+  <dimension ref="A1:AM56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O58" sqref="O58"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1926,36 +2013,311 @@
     <row r="4" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
     </row>
-    <row r="39" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="29:35" x14ac:dyDescent="0.25">
+      <c r="AC20" s="7"/>
+      <c r="AD20" s="7">
+        <v>1</v>
+      </c>
+      <c r="AE20" s="7">
+        <v>2</v>
+      </c>
+      <c r="AF20" s="7">
+        <v>3</v>
+      </c>
+      <c r="AG20" s="7">
+        <v>4</v>
+      </c>
+      <c r="AH20" s="7">
+        <v>5</v>
+      </c>
+      <c r="AI20" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="29:35" x14ac:dyDescent="0.25">
+      <c r="AC21" s="7"/>
+      <c r="AD21" s="7"/>
+      <c r="AE21" s="7"/>
+      <c r="AF21" s="7"/>
+      <c r="AG21" s="7"/>
+      <c r="AH21" s="7"/>
+      <c r="AI21" s="7"/>
+    </row>
+    <row r="22" spans="29:35" x14ac:dyDescent="0.25">
+      <c r="AC22" s="7"/>
+      <c r="AD22" s="7"/>
+      <c r="AE22" s="7"/>
+      <c r="AF22" s="7"/>
+      <c r="AG22" s="7"/>
+      <c r="AH22" s="7"/>
+      <c r="AI22" s="7"/>
+    </row>
+    <row r="23" spans="29:35" x14ac:dyDescent="0.25">
+      <c r="AC23" s="7"/>
+      <c r="AD23" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE23" s="7">
+        <v>1</v>
+      </c>
+      <c r="AF23" s="7">
+        <v>2</v>
+      </c>
+      <c r="AG23" s="7">
+        <v>3</v>
+      </c>
+      <c r="AH23" s="7">
+        <v>4</v>
+      </c>
+      <c r="AI23" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="29:35" x14ac:dyDescent="0.25">
+      <c r="AC24" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD24" s="8"/>
+      <c r="AE24" s="8"/>
+      <c r="AF24" s="8"/>
+      <c r="AG24" s="7"/>
+      <c r="AH24" s="7"/>
+      <c r="AI24" s="7"/>
+    </row>
+    <row r="25" spans="29:35" x14ac:dyDescent="0.25">
+      <c r="AC25" s="7">
+        <v>1</v>
+      </c>
+      <c r="AD25" s="8"/>
+      <c r="AE25" s="8"/>
+      <c r="AF25" s="8"/>
+      <c r="AG25" s="7"/>
+      <c r="AH25" s="7"/>
+      <c r="AI25" s="7"/>
+    </row>
+    <row r="26" spans="29:35" x14ac:dyDescent="0.25">
+      <c r="AC26" s="7">
+        <v>2</v>
+      </c>
+      <c r="AD26" s="8"/>
+      <c r="AE26" s="8"/>
+      <c r="AF26" s="8"/>
+      <c r="AG26" s="7"/>
+      <c r="AH26" s="7"/>
+      <c r="AI26" s="7"/>
+    </row>
+    <row r="27" spans="29:35" x14ac:dyDescent="0.25">
+      <c r="AC27" s="7">
+        <v>3</v>
+      </c>
+      <c r="AD27" s="7"/>
+      <c r="AE27" s="7"/>
+      <c r="AF27" s="7"/>
+      <c r="AG27" s="7"/>
+      <c r="AH27" s="7"/>
+      <c r="AI27" s="7"/>
+    </row>
+    <row r="28" spans="29:35" x14ac:dyDescent="0.25">
+      <c r="AC28" s="7">
+        <v>4</v>
+      </c>
+      <c r="AD28" s="7"/>
+      <c r="AE28" s="7"/>
+      <c r="AF28" s="7"/>
+      <c r="AG28" s="7"/>
+      <c r="AH28" s="7"/>
+      <c r="AI28" s="7"/>
+    </row>
+    <row r="29" spans="29:35" x14ac:dyDescent="0.25">
+      <c r="AC29" s="7">
+        <v>5</v>
+      </c>
+      <c r="AD29" s="7"/>
+      <c r="AE29" s="7"/>
+      <c r="AF29" s="7"/>
+      <c r="AG29" s="7"/>
+      <c r="AH29" s="7"/>
+      <c r="AI29" s="7"/>
+    </row>
+    <row r="30" spans="29:35" x14ac:dyDescent="0.25">
+      <c r="AC30" s="7">
+        <v>6</v>
+      </c>
+      <c r="AD30" s="7"/>
+      <c r="AE30" s="7"/>
+      <c r="AF30" s="7"/>
+      <c r="AG30" s="7"/>
+      <c r="AH30" s="7"/>
+      <c r="AI30" s="7"/>
+    </row>
+    <row r="31" spans="29:35" x14ac:dyDescent="0.25">
+      <c r="AC31" s="7">
+        <v>7</v>
+      </c>
+      <c r="AD31" s="7"/>
+      <c r="AE31" s="7"/>
+      <c r="AF31" s="7"/>
+      <c r="AG31" s="7"/>
+      <c r="AH31" s="7"/>
+      <c r="AI31" s="7"/>
+    </row>
+    <row r="32" spans="29:35" x14ac:dyDescent="0.25">
+      <c r="AC32" s="7">
+        <v>8</v>
+      </c>
+      <c r="AD32" s="7"/>
+      <c r="AE32" s="7"/>
+      <c r="AF32" s="7"/>
+      <c r="AG32" s="7"/>
+      <c r="AH32" s="7"/>
+      <c r="AI32" s="7"/>
+    </row>
+    <row r="33" spans="9:39" x14ac:dyDescent="0.25">
+      <c r="AC33" s="7">
+        <v>8</v>
+      </c>
+      <c r="AD33" s="7"/>
+      <c r="AE33" s="7"/>
+      <c r="AF33" s="7"/>
+      <c r="AG33" s="7"/>
+      <c r="AH33" s="7"/>
+      <c r="AI33" s="7"/>
+    </row>
+    <row r="34" spans="9:39" x14ac:dyDescent="0.25">
+      <c r="AC34" s="7"/>
+      <c r="AD34" s="7"/>
+      <c r="AE34" s="7"/>
+      <c r="AF34" s="7"/>
+      <c r="AG34" s="7"/>
+      <c r="AH34" s="7"/>
+      <c r="AI34" s="7"/>
+    </row>
+    <row r="35" spans="9:39" x14ac:dyDescent="0.25">
+      <c r="AC35" s="7"/>
+      <c r="AD35" s="7"/>
+      <c r="AE35" s="7"/>
+      <c r="AF35" s="7"/>
+      <c r="AG35" s="7"/>
+      <c r="AH35" s="7"/>
+      <c r="AI35" s="7"/>
+    </row>
+    <row r="36" spans="9:39" x14ac:dyDescent="0.25">
+      <c r="AC36" s="7"/>
+      <c r="AD36" s="7"/>
+      <c r="AE36" s="7"/>
+      <c r="AF36" s="7"/>
+      <c r="AG36" s="7"/>
+      <c r="AH36" s="7"/>
+      <c r="AI36" s="7"/>
+    </row>
+    <row r="37" spans="9:39" x14ac:dyDescent="0.25">
+      <c r="AC37" s="7"/>
+      <c r="AD37" s="7"/>
+      <c r="AE37" s="7"/>
+      <c r="AF37" s="7"/>
+      <c r="AG37" s="7"/>
+      <c r="AH37" s="7"/>
+      <c r="AI37" s="7"/>
+    </row>
+    <row r="38" spans="9:39" x14ac:dyDescent="0.25">
+      <c r="AC38" s="7"/>
+      <c r="AD38" s="7"/>
+      <c r="AE38" s="7"/>
+      <c r="AF38" s="7"/>
+      <c r="AG38" s="7"/>
+      <c r="AH38" s="7"/>
+      <c r="AI38" s="7"/>
+    </row>
+    <row r="39" spans="9:39" x14ac:dyDescent="0.25">
       <c r="I39" s="2"/>
-    </row>
-    <row r="40" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="AC39" s="7"/>
+      <c r="AD39" s="7"/>
+      <c r="AE39" s="7"/>
+      <c r="AF39" s="7"/>
+      <c r="AG39" s="7"/>
+      <c r="AH39" s="7"/>
+      <c r="AI39" s="7"/>
+    </row>
+    <row r="40" spans="9:39" x14ac:dyDescent="0.25">
       <c r="I40" s="2"/>
-    </row>
-    <row r="41" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="AC40" s="7"/>
+      <c r="AD40" s="7"/>
+      <c r="AE40" s="7"/>
+      <c r="AF40" s="7"/>
+      <c r="AG40" s="7"/>
+      <c r="AH40" s="7"/>
+      <c r="AI40" s="7"/>
+    </row>
+    <row r="41" spans="9:39" x14ac:dyDescent="0.25">
       <c r="I41" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="AC41" s="7"/>
+      <c r="AD41" s="7"/>
+      <c r="AE41" s="7"/>
+      <c r="AF41" s="7"/>
+      <c r="AG41" s="7"/>
+      <c r="AH41" s="7"/>
+      <c r="AI41" s="7"/>
+      <c r="AJ41" s="7"/>
+      <c r="AK41" s="7"/>
+      <c r="AL41" s="7"/>
+      <c r="AM41" s="7"/>
+    </row>
+    <row r="42" spans="9:39" x14ac:dyDescent="0.25">
+      <c r="AC42" s="7"/>
+      <c r="AD42" s="7"/>
+      <c r="AE42" s="7"/>
+      <c r="AF42" s="7"/>
+      <c r="AG42" s="7"/>
+      <c r="AH42" s="7"/>
+      <c r="AI42" s="7"/>
+      <c r="AJ42" s="7"/>
+      <c r="AK42" s="7"/>
+      <c r="AL42" s="7"/>
+      <c r="AM42" s="7"/>
+    </row>
+    <row r="43" spans="9:39" x14ac:dyDescent="0.25">
       <c r="I43" s="4" t="s">
         <v>3</v>
       </c>
       <c r="P43" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="44" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="AC43" s="7"/>
+      <c r="AD43" s="7"/>
+      <c r="AE43" s="7"/>
+      <c r="AF43" s="7"/>
+      <c r="AG43" s="7"/>
+      <c r="AH43" s="7"/>
+      <c r="AI43" s="7"/>
+      <c r="AJ43" s="7"/>
+      <c r="AK43" s="7"/>
+      <c r="AL43" s="7"/>
+      <c r="AM43" s="7"/>
+    </row>
+    <row r="44" spans="9:39" x14ac:dyDescent="0.25">
       <c r="I44" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="AC44" s="7"/>
+      <c r="AD44" s="7"/>
+      <c r="AE44" s="7"/>
+      <c r="AF44" s="7"/>
+      <c r="AG44" s="7"/>
+      <c r="AH44" s="7"/>
+      <c r="AI44" s="7"/>
+      <c r="AJ44" s="7"/>
+      <c r="AK44" s="7"/>
+      <c r="AL44" s="7"/>
+      <c r="AM44" s="7"/>
+    </row>
+    <row r="45" spans="9:39" x14ac:dyDescent="0.25">
       <c r="I45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="9:39" x14ac:dyDescent="0.25">
       <c r="I47" s="4" t="s">
         <v>13</v>
       </c>
@@ -1963,34 +2325,45 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="9:39" x14ac:dyDescent="0.25">
       <c r="I48" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="9:25" x14ac:dyDescent="0.25">
       <c r="I50" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="P50" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="9:25" x14ac:dyDescent="0.25">
       <c r="I51" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="9:25" x14ac:dyDescent="0.25">
       <c r="I52" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="9:25" x14ac:dyDescent="0.25">
       <c r="I53" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="9:25" x14ac:dyDescent="0.25">
       <c r="I55" s="4" t="s">
         <v>9</v>
+      </c>
+      <c r="X55" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="9:25" x14ac:dyDescent="0.25">
+      <c r="Y56" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on OOP approach. Ticking off procedural approach items and rewording
</commit_message>
<xml_diff>
--- a/Design Brief and Analysis/SnapperCodingChallengeDesignDocument.xlsx
+++ b/Design Brief and Analysis/SnapperCodingChallengeDesignDocument.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcox\Desktop\git\SnapperCodingChallenge\Design Brief and Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9554C22-758A-4CA3-813D-09C202679C32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD426F77-BDAD-4B6D-8A7A-48B120298C6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DesignBrief" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t xml:space="preserve">Snapper Coding Challenge </t>
   </si>
@@ -156,6 +156,12 @@
   <si>
     <t>`</t>
   </si>
+  <si>
+    <t>TODO:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Exception handling when grid is not rectangular </t>
+  </si>
 </sst>
 </file>
 
@@ -218,18 +224,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -244,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -253,9 +253,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -678,15 +675,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>72838</xdr:rowOff>
+      <xdr:colOff>81642</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>140873</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>149678</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>367392</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -701,8 +698,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4898571" y="3461017"/>
-          <a:ext cx="5031922" cy="3124840"/>
+          <a:off x="4980213" y="4168587"/>
+          <a:ext cx="7728858" cy="5057056"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -756,34 +753,104 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" u="none" baseline="0"/>
+            <a:t>Yes, we will do this in our OOP approach. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
             <a:t>2. Should we use 2d-array [][] or jagged array [,] - working with rectangular objects so 2d-array will be used as no need for flexibility of width of rows etc. </a:t>
           </a:r>
         </a:p>
         <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" u="none" baseline="0"/>
+            <a:t>Use multi-dimensional arrays - we should assume that all rows and columns of characters defined in the datafile to be equal. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
             <a:t>3. We should error handle to catch when grid not rectangular and there are errors. </a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" u="none" baseline="0"/>
+            <a:t>Done. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
             <a:t>4. The objects contain empty white columns and rows - we should trim these out to optimise the algorithm. </a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1. Exception handling when grid is not rectangular </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" b="1"/>
+            <a:t>DONE. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
             <a:t>5. What happens if the input files contains other non "X" or white-space ASCII characters? Do we want tight or loose exception handling - e.g. return errror message if contaisn non "X" characters, or simply run through analysis and assume that if not X, not counted as data. </a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" u="none" baseline="0"/>
+            <a:t>DONE</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
-            <a:t>6. Do a simple method for a grid of say 4 1's within 16*16 grid as a practice!</a:t>
-          </a:r>
+            <a:t>6. Do a simple method for a grid of say 4 1's within 16*16 grid as a practice! </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" u="none" baseline="0"/>
+            <a:t>DONE - extensive unit testing. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
         </a:p>
         <a:p>
           <a:r>
@@ -793,12 +860,24 @@
         </a:p>
         <a:p>
           <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" u="none" baseline="0"/>
+            <a:t>Hasnt seem to be an issue </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="1" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
             <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
             <a:t>8. How are the "co-ordinates" of the ITarget defined? </a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" u="none" baseline="0"/>
+            <a:t>Global coordinates, based on the centroid of the target object/array. </a:t>
+          </a:r>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-GB" sz="1100" b="1"/>
@@ -817,8 +896,8 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>40822</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -833,8 +912,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="200025" y="6992419"/>
-          <a:ext cx="4273924" cy="5726257"/>
+          <a:off x="200025" y="8016957"/>
+          <a:ext cx="4324350" cy="5386079"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1217,25 +1296,6 @@
             </a:rPr>
             <a:t>1. Write a method to compare a given matrix with another matrix, comparing ONLY against a given list of co-ordinates</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
           <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
             <a:solidFill>
               <a:schemeClr val="dk1"/>
@@ -1293,7 +1353,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
+            <a:rPr lang="en-GB" sz="1100" b="1" u="none" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -1323,6 +1383,65 @@
             <a:tabLst/>
             <a:defRPr/>
           </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" b="1" u="none" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" u="sng" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Post-Processing </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
           <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
             <a:solidFill>
               <a:schemeClr val="dk1"/>
@@ -1352,7 +1471,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" u="sng" baseline="0">
+            <a:rPr lang="en-GB" sz="1100" b="1" u="none" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -1361,7 +1480,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Post-Processing </a:t>
+            <a:t>1. Print to console when a starship has been detected, along with its coordinates and target accuracy =&gt; the coordinates should be defined as the centroid of the 2D Array </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1410,37 +1529,6 @@
             <a:tabLst/>
             <a:defRPr/>
           </a:pPr>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>1. Print to console when a starship has been detected, along with its coordinates and target accuracy =&gt; the coordinates should be defined as the centroid of the 2D Array </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
           <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
             <a:solidFill>
               <a:schemeClr val="dk1"/>
@@ -1469,37 +1557,6 @@
             <a:tabLst/>
             <a:defRPr/>
           </a:pPr>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>2. (If get time =&gt; print out the map, and shade in yellow where a spaceship has been identified and orange for nuclear torpedeoes for fun). </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
           <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
             <a:solidFill>
               <a:schemeClr val="dk1"/>
@@ -1556,90 +1613,6 @@
             <a:tabLst/>
             <a:defRPr/>
           </a:pPr>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
           <a:endParaRPr lang="en-GB" u="none">
             <a:effectLst/>
           </a:endParaRPr>
@@ -1672,50 +1645,6 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>43</xdr:col>
-      <xdr:colOff>462306</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20AADD9B-62CC-42D4-88BF-E4D5DDBE6DA9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10695214" y="4789714"/>
-          <a:ext cx="16804485" cy="8191500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1984,10 +1913,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM56"/>
+  <dimension ref="A1:AM61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1995,311 +1924,53 @@
     <col min="9" max="9" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:22" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:22" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:22" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:22" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
     </row>
-    <row r="20" spans="29:35" x14ac:dyDescent="0.25">
-      <c r="AC20" s="7"/>
-      <c r="AD20" s="7">
-        <v>1</v>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V8" s="2" t="s">
+        <v>16</v>
       </c>
-      <c r="AE20" s="7">
-        <v>2</v>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V10" t="s">
+        <v>17</v>
       </c>
-      <c r="AF20" s="7">
-        <v>3</v>
-      </c>
-      <c r="AG20" s="7">
-        <v>4</v>
-      </c>
-      <c r="AH20" s="7">
-        <v>5</v>
-      </c>
-      <c r="AI20" s="7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="29:35" x14ac:dyDescent="0.25">
-      <c r="AC21" s="7"/>
-      <c r="AD21" s="7"/>
-      <c r="AE21" s="7"/>
-      <c r="AF21" s="7"/>
-      <c r="AG21" s="7"/>
-      <c r="AH21" s="7"/>
-      <c r="AI21" s="7"/>
-    </row>
-    <row r="22" spans="29:35" x14ac:dyDescent="0.25">
-      <c r="AC22" s="7"/>
-      <c r="AD22" s="7"/>
-      <c r="AE22" s="7"/>
-      <c r="AF22" s="7"/>
-      <c r="AG22" s="7"/>
-      <c r="AH22" s="7"/>
-      <c r="AI22" s="7"/>
-    </row>
-    <row r="23" spans="29:35" x14ac:dyDescent="0.25">
-      <c r="AC23" s="7"/>
-      <c r="AD23" s="7">
-        <v>0</v>
-      </c>
-      <c r="AE23" s="7">
-        <v>1</v>
-      </c>
-      <c r="AF23" s="7">
-        <v>2</v>
-      </c>
-      <c r="AG23" s="7">
-        <v>3</v>
-      </c>
-      <c r="AH23" s="7">
-        <v>4</v>
-      </c>
-      <c r="AI23" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="29:35" x14ac:dyDescent="0.25">
-      <c r="AC24" s="7">
-        <v>0</v>
-      </c>
-      <c r="AD24" s="8"/>
-      <c r="AE24" s="8"/>
-      <c r="AF24" s="8"/>
-      <c r="AG24" s="7"/>
-      <c r="AH24" s="7"/>
-      <c r="AI24" s="7"/>
-    </row>
-    <row r="25" spans="29:35" x14ac:dyDescent="0.25">
-      <c r="AC25" s="7">
-        <v>1</v>
-      </c>
-      <c r="AD25" s="8"/>
-      <c r="AE25" s="8"/>
-      <c r="AF25" s="8"/>
-      <c r="AG25" s="7"/>
-      <c r="AH25" s="7"/>
-      <c r="AI25" s="7"/>
-    </row>
-    <row r="26" spans="29:35" x14ac:dyDescent="0.25">
-      <c r="AC26" s="7">
-        <v>2</v>
-      </c>
-      <c r="AD26" s="8"/>
-      <c r="AE26" s="8"/>
-      <c r="AF26" s="8"/>
-      <c r="AG26" s="7"/>
-      <c r="AH26" s="7"/>
-      <c r="AI26" s="7"/>
-    </row>
-    <row r="27" spans="29:35" x14ac:dyDescent="0.25">
-      <c r="AC27" s="7">
-        <v>3</v>
-      </c>
-      <c r="AD27" s="7"/>
-      <c r="AE27" s="7"/>
-      <c r="AF27" s="7"/>
-      <c r="AG27" s="7"/>
-      <c r="AH27" s="7"/>
-      <c r="AI27" s="7"/>
-    </row>
-    <row r="28" spans="29:35" x14ac:dyDescent="0.25">
-      <c r="AC28" s="7">
-        <v>4</v>
-      </c>
-      <c r="AD28" s="7"/>
-      <c r="AE28" s="7"/>
-      <c r="AF28" s="7"/>
-      <c r="AG28" s="7"/>
-      <c r="AH28" s="7"/>
-      <c r="AI28" s="7"/>
-    </row>
-    <row r="29" spans="29:35" x14ac:dyDescent="0.25">
-      <c r="AC29" s="7">
-        <v>5</v>
-      </c>
-      <c r="AD29" s="7"/>
-      <c r="AE29" s="7"/>
-      <c r="AF29" s="7"/>
-      <c r="AG29" s="7"/>
-      <c r="AH29" s="7"/>
-      <c r="AI29" s="7"/>
-    </row>
-    <row r="30" spans="29:35" x14ac:dyDescent="0.25">
-      <c r="AC30" s="7">
-        <v>6</v>
-      </c>
-      <c r="AD30" s="7"/>
-      <c r="AE30" s="7"/>
-      <c r="AF30" s="7"/>
-      <c r="AG30" s="7"/>
-      <c r="AH30" s="7"/>
-      <c r="AI30" s="7"/>
-    </row>
-    <row r="31" spans="29:35" x14ac:dyDescent="0.25">
-      <c r="AC31" s="7">
-        <v>7</v>
-      </c>
-      <c r="AD31" s="7"/>
-      <c r="AE31" s="7"/>
-      <c r="AF31" s="7"/>
-      <c r="AG31" s="7"/>
-      <c r="AH31" s="7"/>
-      <c r="AI31" s="7"/>
-    </row>
-    <row r="32" spans="29:35" x14ac:dyDescent="0.25">
-      <c r="AC32" s="7">
-        <v>8</v>
-      </c>
-      <c r="AD32" s="7"/>
-      <c r="AE32" s="7"/>
-      <c r="AF32" s="7"/>
-      <c r="AG32" s="7"/>
-      <c r="AH32" s="7"/>
-      <c r="AI32" s="7"/>
-    </row>
-    <row r="33" spans="9:39" x14ac:dyDescent="0.25">
-      <c r="AC33" s="7">
-        <v>8</v>
-      </c>
-      <c r="AD33" s="7"/>
-      <c r="AE33" s="7"/>
-      <c r="AF33" s="7"/>
-      <c r="AG33" s="7"/>
-      <c r="AH33" s="7"/>
-      <c r="AI33" s="7"/>
-    </row>
-    <row r="34" spans="9:39" x14ac:dyDescent="0.25">
-      <c r="AC34" s="7"/>
-      <c r="AD34" s="7"/>
-      <c r="AE34" s="7"/>
-      <c r="AF34" s="7"/>
-      <c r="AG34" s="7"/>
-      <c r="AH34" s="7"/>
-      <c r="AI34" s="7"/>
-    </row>
-    <row r="35" spans="9:39" x14ac:dyDescent="0.25">
-      <c r="AC35" s="7"/>
-      <c r="AD35" s="7"/>
-      <c r="AE35" s="7"/>
-      <c r="AF35" s="7"/>
-      <c r="AG35" s="7"/>
-      <c r="AH35" s="7"/>
-      <c r="AI35" s="7"/>
-    </row>
-    <row r="36" spans="9:39" x14ac:dyDescent="0.25">
-      <c r="AC36" s="7"/>
-      <c r="AD36" s="7"/>
-      <c r="AE36" s="7"/>
-      <c r="AF36" s="7"/>
-      <c r="AG36" s="7"/>
-      <c r="AH36" s="7"/>
-      <c r="AI36" s="7"/>
-    </row>
-    <row r="37" spans="9:39" x14ac:dyDescent="0.25">
-      <c r="AC37" s="7"/>
-      <c r="AD37" s="7"/>
-      <c r="AE37" s="7"/>
-      <c r="AF37" s="7"/>
-      <c r="AG37" s="7"/>
-      <c r="AH37" s="7"/>
-      <c r="AI37" s="7"/>
-    </row>
-    <row r="38" spans="9:39" x14ac:dyDescent="0.25">
-      <c r="AC38" s="7"/>
-      <c r="AD38" s="7"/>
-      <c r="AE38" s="7"/>
-      <c r="AF38" s="7"/>
-      <c r="AG38" s="7"/>
-      <c r="AH38" s="7"/>
-      <c r="AI38" s="7"/>
     </row>
     <row r="39" spans="9:39" x14ac:dyDescent="0.25">
       <c r="I39" s="2"/>
-      <c r="AC39" s="7"/>
-      <c r="AD39" s="7"/>
-      <c r="AE39" s="7"/>
-      <c r="AF39" s="7"/>
-      <c r="AG39" s="7"/>
-      <c r="AH39" s="7"/>
-      <c r="AI39" s="7"/>
-    </row>
-    <row r="40" spans="9:39" x14ac:dyDescent="0.25">
-      <c r="I40" s="2"/>
-      <c r="AC40" s="7"/>
-      <c r="AD40" s="7"/>
-      <c r="AE40" s="7"/>
-      <c r="AF40" s="7"/>
-      <c r="AG40" s="7"/>
-      <c r="AH40" s="7"/>
-      <c r="AI40" s="7"/>
     </row>
     <row r="41" spans="9:39" x14ac:dyDescent="0.25">
-      <c r="I41" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC41" s="7"/>
-      <c r="AD41" s="7"/>
-      <c r="AE41" s="7"/>
-      <c r="AF41" s="7"/>
-      <c r="AG41" s="7"/>
-      <c r="AH41" s="7"/>
-      <c r="AI41" s="7"/>
-      <c r="AJ41" s="7"/>
       <c r="AK41" s="7"/>
       <c r="AL41" s="7"/>
       <c r="AM41" s="7"/>
     </row>
     <row r="42" spans="9:39" x14ac:dyDescent="0.25">
-      <c r="AC42" s="7"/>
-      <c r="AD42" s="7"/>
-      <c r="AE42" s="7"/>
-      <c r="AF42" s="7"/>
-      <c r="AG42" s="7"/>
-      <c r="AH42" s="7"/>
-      <c r="AI42" s="7"/>
-      <c r="AJ42" s="7"/>
       <c r="AK42" s="7"/>
       <c r="AL42" s="7"/>
       <c r="AM42" s="7"/>
     </row>
     <row r="43" spans="9:39" x14ac:dyDescent="0.25">
-      <c r="I43" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P43" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC43" s="7"/>
-      <c r="AD43" s="7"/>
-      <c r="AE43" s="7"/>
-      <c r="AF43" s="7"/>
-      <c r="AG43" s="7"/>
-      <c r="AH43" s="7"/>
-      <c r="AI43" s="7"/>
-      <c r="AJ43" s="7"/>
       <c r="AK43" s="7"/>
       <c r="AL43" s="7"/>
       <c r="AM43" s="7"/>
     </row>
     <row r="44" spans="9:39" x14ac:dyDescent="0.25">
-      <c r="I44" t="s">
-        <v>2</v>
-      </c>
       <c r="AC44" s="7"/>
       <c r="AD44" s="7"/>
       <c r="AE44" s="7"/>
@@ -2312,58 +1983,77 @@
       <c r="AL44" s="7"/>
       <c r="AM44" s="7"/>
     </row>
-    <row r="45" spans="9:39" x14ac:dyDescent="0.25">
-      <c r="I45" t="s">
+    <row r="46" spans="9:39" x14ac:dyDescent="0.25">
+      <c r="I46" s="2"/>
+    </row>
+    <row r="47" spans="9:39" x14ac:dyDescent="0.25">
+      <c r="I47" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="9:25" x14ac:dyDescent="0.25">
+      <c r="I49" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P49" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="9:25" x14ac:dyDescent="0.25">
+      <c r="I50" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="9:25" x14ac:dyDescent="0.25">
+      <c r="I51" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="9:39" x14ac:dyDescent="0.25">
-      <c r="I47" s="4" t="s">
+    <row r="53" spans="9:25" x14ac:dyDescent="0.25">
+      <c r="I53" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P47" s="2" t="s">
+      <c r="P53" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="9:39" x14ac:dyDescent="0.25">
-      <c r="I48" t="s">
+    <row r="54" spans="9:25" x14ac:dyDescent="0.25">
+      <c r="I54" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="9:25" x14ac:dyDescent="0.25">
-      <c r="I50" s="4" t="s">
+    <row r="56" spans="9:25" x14ac:dyDescent="0.25">
+      <c r="I56" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="P50" s="2" t="s">
+      <c r="P56" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="51" spans="9:25" x14ac:dyDescent="0.25">
-      <c r="I51" t="s">
+      <c r="Y56" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="9:25" x14ac:dyDescent="0.25">
+      <c r="I57" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="9:25" x14ac:dyDescent="0.25">
-      <c r="I52" s="3" t="s">
+    <row r="58" spans="9:25" x14ac:dyDescent="0.25">
+      <c r="I58" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="9:25" x14ac:dyDescent="0.25">
-      <c r="I53" s="3" t="s">
+    <row r="59" spans="9:25" x14ac:dyDescent="0.25">
+      <c r="I59" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="9:25" x14ac:dyDescent="0.25">
-      <c r="I55" s="4" t="s">
+    <row r="61" spans="9:25" x14ac:dyDescent="0.25">
+      <c r="I61" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="X55" s="2" t="s">
+      <c r="X61" s="2" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="56" spans="9:25" x14ac:dyDescent="0.25">
-      <c r="Y56" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wrote up console application requirements.
</commit_message>
<xml_diff>
--- a/Design Brief and Analysis/SnapperCodingChallengeDesignDocument.xlsx
+++ b/Design Brief and Analysis/SnapperCodingChallengeDesignDocument.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcox\Desktop\git\SnapperCodingChallenge\Design Brief and Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F20C711-4B12-48A3-B71C-33F7B078760C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33414C9-10B2-4A0A-BD95-D29D275E3AB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6810" yWindow="-330" windowWidth="7500" windowHeight="6000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DesignBrief" sheetId="1" r:id="rId1"/>
@@ -155,10 +155,10 @@
     <t>`</t>
   </si>
   <si>
-    <t xml:space="preserve">Object-Orientated Approach V1.0 </t>
+    <t>DONE</t>
   </si>
   <si>
-    <t>DONE</t>
+    <t>\</t>
   </si>
 </sst>
 </file>
@@ -1653,15 +1653,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>97572</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>75400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>367393</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>10406</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1676,8 +1676,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="304800" y="1800225"/>
-          <a:ext cx="7105650" cy="5581650"/>
+          <a:off x="97572" y="1286436"/>
+          <a:ext cx="5780714" cy="7364506"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1712,148 +1712,7 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1"/>
-            <a:t>Nouns: </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-            <a:t>Spaceships and Torpedos - Targets that are to be detected/ </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-            <a:t>Snapper Image - Map data to be scanned. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-            <a:t>PercentageAccuracy - the accuracy we are working to. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-            <a:t>Logger - we need somewhere to log to e.g. the console. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-            <a:t>The following procedure will be used to operate the "Scanner". For now focus on getting a first draft on - we will refactor later to make remove dependencies and make the program more extensible in the future. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
-            <a:t>Setting up the scanner. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-            <a:t>1. "Turn on" (or rather instantiate an instance of the scanner). </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-            <a:t>2.  Inject an ILogger object =&gt; this will be used to log our findings. For the time being will only deal with logging to the console, but we should allow flexibility to write to a logfile/textdump etc - it will contain only a single method WriteMessage()</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-            <a:t>3. Inject an ISnapperImage Object =&gt; this implements an interface containing only a single method, which returns a 2d array of characters for us to work with (in our case our data entry is in the form of a textfile, but in the future we should make this extensible to deal with HTTP requests, DBs etc....</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
-            <a:t>Operating the Scanner. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" u="sng" baseline="0"/>
-            <a:t>Methods: </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="sng" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
-            <a:t>public void </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-            <a:t>3. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-            <a:t>3. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0">
+            <a:rPr lang="en-GB" sz="1100" b="1" i="0" u="none" strike="noStrike">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -1862,42 +1721,149 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Specify the precision of the scanner as a double (0.5 = 50%)</a:t>
+            <a:t>User Interface </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB"/>
+            <a:t> </a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0"/>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-            <a:t>Supply the ISnapperImage object =&gt; this will only require a single method which gives as a 2D array to work with, this could come from a textfile, MongoDB, HTTP request etc etc.....</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="sng" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="1"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="1" u="none" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="1" u="none" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="1" u="none" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="1"/>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>Lets think about exactly how such a program would operate once it has been developed to be used by someone. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>1. We're handed a "snapper" image i.e. textfile we want to load into the program.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>2. We "load" into the program the elements we're checking against. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>3. We run the solver, which echoes the progress to the Console</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>4. We examine the output file which records the following in a neat table:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>===========</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>SNAPPER OUPUT </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>Date: </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>===========</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>Options: </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>MinimumAccyracy = 0.5 (or 50%)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>Target Summary; </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>Name: Starship</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>Instances: 4 (for example</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>Coordinates:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>(32, 45)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>(23, 43)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>(21, 20)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>(80, 90)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2171,8 +2137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U6" sqref="U6:AA11"/>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W25" sqref="W25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2245,7 +2211,7 @@
         <v>3</v>
       </c>
       <c r="P49" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="50" spans="9:25" x14ac:dyDescent="0.25">
@@ -2263,7 +2229,7 @@
         <v>13</v>
       </c>
       <c r="P53" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="54" spans="9:25" x14ac:dyDescent="0.25">
@@ -2276,7 +2242,7 @@
         <v>4</v>
       </c>
       <c r="P56" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Y56" t="s">
         <v>14</v>
@@ -2302,7 +2268,7 @@
         <v>9</v>
       </c>
       <c r="X61" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2314,10 +2280,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2C6159A-D54A-4699-848D-469CF142CB07}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U22" sqref="U22"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R26" sqref="R26:R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2337,9 +2303,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>15</v>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+    </row>
+    <row r="26" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R26" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalised OOP approach. Added OOP unit tests.
</commit_message>
<xml_diff>
--- a/Design Brief and Analysis/SnapperCodingChallengeDesignDocument.xlsx
+++ b/Design Brief and Analysis/SnapperCodingChallengeDesignDocument.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcox\Desktop\git\SnapperCodingChallenge\Design Brief and Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCF058D-5363-4C3C-8626-1D12C0D639EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7B051C-C342-4D02-A882-815B8F5A346D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19110" yWindow="0" windowWidth="7500" windowHeight="6000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DesignBrief" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
   <si>
     <t xml:space="preserve">Snapper Coding Challenge </t>
   </si>
@@ -193,19 +193,22 @@
     <t>NOTATION</t>
   </si>
   <si>
-    <t>x =&gt;</t>
-  </si>
-  <si>
     <t>X</t>
-  </si>
-  <si>
-    <t>y</t>
   </si>
   <si>
     <t>v</t>
   </si>
   <si>
     <t>||</t>
+  </si>
+  <si>
+    <t>TODO List</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y =&gt;</t>
   </si>
 </sst>
 </file>
@@ -2698,7 +2701,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" baseline="0"/>
-            <a:t>1. The GridRepresentaton of a SnapperImage, Target etc is defined as [col,rows]. </a:t>
+            <a:t>1. The GridRepresentaton of a SnapperImage, Target etc is defined as [rows,cols]</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2861,8 +2864,8 @@
       <xdr:rowOff>41063</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>264940</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>44823</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>176893</xdr:rowOff>
     </xdr:to>
@@ -2879,8 +2882,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6838871" y="4613063"/>
-          <a:ext cx="5441176" cy="3755330"/>
+          <a:off x="6759629" y="4613063"/>
+          <a:ext cx="2720547" cy="3755330"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2989,6 +2992,50 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>392748</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>189952</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{249D87EE-F858-4C55-B1C7-EBE3CA0FCBAD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12864353" y="1905000"/>
+          <a:ext cx="4628571" cy="4380952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3492,10 +3539,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FD2C6B0-35FC-4C92-8DCB-A58CE79CB204}">
-  <dimension ref="A1:AA27"/>
+  <dimension ref="A1:AC27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3504,15 +3551,15 @@
     <col min="13" max="27" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="O1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="L3" s="2" t="s">
         <v>24</v>
       </c>
@@ -3525,7 +3572,7 @@
         <v>1</v>
       </c>
       <c r="Q3" s="11">
-        <f t="shared" ref="Q3:Y3" si="0">P3+1</f>
+        <f t="shared" ref="Q3:X3" si="0">P3+1</f>
         <v>2</v>
       </c>
       <c r="R3" s="11">
@@ -3560,7 +3607,7 @@
       <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="N4" s="11">
         <v>0</v>
       </c>
@@ -3575,9 +3622,9 @@
       <c r="W4" s="10"/>
       <c r="X4" s="10"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="M5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="N5" s="11">
         <v>1</v>
@@ -3592,10 +3639,13 @@
       <c r="V5" s="10"/>
       <c r="W5" s="10"/>
       <c r="X5" s="10"/>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="M6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N6" s="11">
         <v>2</v>
@@ -3605,19 +3655,19 @@
       <c r="Q6" s="12"/>
       <c r="R6" s="13"/>
       <c r="S6" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="T6" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U6" s="14"/>
       <c r="V6" s="10"/>
       <c r="W6" s="10"/>
       <c r="X6" s="10"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="M7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N7" s="11">
         <v>3</v>
@@ -3626,22 +3676,22 @@
       <c r="P7" s="10"/>
       <c r="Q7" s="10"/>
       <c r="R7" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S7" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="T7" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U7" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="V7" s="10"/>
       <c r="W7" s="10"/>
       <c r="X7" s="10"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="N8" s="11">
         <v>4</v>
       </c>
@@ -3650,17 +3700,17 @@
       <c r="Q8" s="10"/>
       <c r="R8" s="14"/>
       <c r="S8" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="T8" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U8" s="14"/>
       <c r="V8" s="10"/>
       <c r="W8" s="10"/>
       <c r="X8" s="10"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="N9" s="11">
         <v>5</v>
       </c>
@@ -3669,17 +3719,17 @@
       <c r="Q9" s="10"/>
       <c r="R9" s="14"/>
       <c r="S9" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="T9" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U9" s="14"/>
       <c r="V9" s="10"/>
       <c r="W9" s="10"/>
       <c r="X9" s="10"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="N10" s="11">
         <v>6</v>
       </c>
@@ -3687,22 +3737,22 @@
       <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
       <c r="R10" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S10" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="T10" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U10" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="V10" s="10"/>
       <c r="W10" s="10"/>
       <c r="X10" s="10"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="N11" s="11">
         <v>7</v>
       </c>
@@ -3717,7 +3767,7 @@
       <c r="W11" s="10"/>
       <c r="X11" s="10"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="N12" s="11">
         <v>8</v>
       </c>
@@ -3732,7 +3782,7 @@
       <c r="W12" s="10"/>
       <c r="X12" s="10"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="N13" s="11">
         <v>9</v>
       </c>
@@ -3747,7 +3797,7 @@
       <c r="W13" s="10"/>
       <c r="X13" s="10"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="N14" s="11"/>
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
@@ -3760,10 +3810,10 @@
       <c r="W14" s="10"/>
       <c r="X14" s="10"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="N15" s="9"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="N16" s="9"/>
     </row>
     <row r="17" spans="14:14" x14ac:dyDescent="0.25">

</xml_diff>